<commit_message>
Added pictures and ensured formatting is uniformed throughout webpage.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF238C6-FAE2-534B-A4E5-F289EB099691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0C0786-2E32-D444-BCA4-824305D40BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="9" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -3810,7 +3810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76825C-C293-7549-99D8-78EF98420F3C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4533,9 +4533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
   <dimension ref="A1:S109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24:D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10175,20 +10175,122 @@
       <c r="A106" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B106" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B107" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="9">
+        <v>0</v>
+      </c>
+      <c r="F107" s="9">
+        <v>0</v>
+      </c>
+      <c r="G107" s="9">
+        <v>0</v>
+      </c>
+      <c r="H107" s="9">
+        <v>0</v>
+      </c>
+      <c r="I107" s="9">
+        <v>0</v>
+      </c>
+      <c r="J107" s="9">
+        <v>0</v>
+      </c>
+      <c r="K107" s="9">
+        <v>0</v>
+      </c>
+      <c r="L107" s="9">
+        <v>0</v>
+      </c>
+      <c r="M107" s="9">
+        <v>0</v>
+      </c>
+      <c r="N107" s="9">
+        <v>0</v>
+      </c>
+      <c r="O107" s="9">
+        <v>0</v>
+      </c>
+      <c r="P107" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q107" s="9">
+        <v>0</v>
+      </c>
+      <c r="R107" s="9">
+        <v>0</v>
+      </c>
+      <c r="S107" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B108" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="9">
+        <v>0</v>
+      </c>
+      <c r="F109" s="9">
+        <v>0</v>
+      </c>
+      <c r="G109" s="9">
+        <v>0</v>
+      </c>
+      <c r="H109" s="9">
+        <v>0</v>
+      </c>
+      <c r="I109" s="9">
+        <v>0</v>
+      </c>
+      <c r="J109" s="9">
+        <v>0</v>
+      </c>
+      <c r="K109" s="9">
+        <v>0</v>
+      </c>
+      <c r="L109" s="9">
+        <v>0</v>
+      </c>
+      <c r="M109" s="9">
+        <v>0</v>
+      </c>
+      <c r="N109" s="9">
+        <v>0</v>
+      </c>
+      <c r="O109" s="9">
+        <v>0</v>
+      </c>
+      <c r="P109" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="9">
+        <v>0</v>
+      </c>
+      <c r="R109" s="9">
+        <v>0</v>
+      </c>
+      <c r="S109" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-updated picture of Aa on substrate and fixed typo for Th.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0C0786-2E32-D444-BCA4-824305D40BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B1052-2EE3-7549-874D-0B07A3FB2652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
@@ -4534,8 +4534,8 @@
   <dimension ref="A1:S109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O21" s="10">
         <v>0</v>
@@ -8593,7 +8593,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M69" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
Added new sites to map of all sites.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B1052-2EE3-7549-874D-0B07A3FB2652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBA00AE-FAB5-C44A-8390-79B06ECBA32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Dr</t>
-  </si>
-  <si>
-    <t>OS</t>
   </si>
   <si>
     <t>Cb</t>
@@ -543,9 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AA6257-4E63-BE4C-BA67-DCDA03B0201E}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C84" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3182,7 +3181,7 @@
         <v>59.7</v>
       </c>
       <c r="E88" s="4">
-        <f t="shared" ref="E88:E94" si="14">B88+C88/60+D88/3600</f>
+        <f t="shared" ref="E88:E95" si="14">B88+C88/60+D88/3600</f>
         <v>29.983249999999998</v>
       </c>
       <c r="F88" s="1">
@@ -3195,7 +3194,7 @@
         <v>25.1</v>
       </c>
       <c r="I88">
-        <f t="shared" ref="I88:I94" si="15">-F88-G88/60-H88/3600</f>
+        <f t="shared" ref="I88:I95" si="15">-F88-G88/60-H88/3600</f>
         <v>-90.090305555555545</v>
       </c>
     </row>
@@ -3247,8 +3246,8 @@
         <f t="shared" si="14"/>
         <v>30.207249999999998</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>20</v>
+      <c r="F90" s="1">
+        <v>90</v>
       </c>
       <c r="G90">
         <v>25</v>
@@ -3256,9 +3255,9 @@
       <c r="H90">
         <v>21.7</v>
       </c>
-      <c r="I90" t="e">
+      <c r="I90">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>-90.422694444444446</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3385,420 +3384,749 @@
         <v>-90.115638888888881</v>
       </c>
     </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" s="1">
+        <v>29</v>
+      </c>
+      <c r="C95">
+        <v>52</v>
+      </c>
+      <c r="D95">
+        <v>0.3</v>
+      </c>
+      <c r="E95" s="4">
+        <f t="shared" si="14"/>
+        <v>29.86675</v>
+      </c>
+      <c r="F95" s="1">
+        <v>90</v>
+      </c>
+      <c r="G95">
+        <v>32</v>
+      </c>
+      <c r="H95">
+        <v>27.411999999999999</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="15"/>
+        <v>-90.540947777777774</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1">
+        <v>30</v>
+      </c>
+      <c r="C97">
+        <v>27</v>
+      </c>
+      <c r="D97">
+        <v>23.4</v>
+      </c>
+      <c r="E97" s="4">
+        <f t="shared" ref="E97:E116" si="16">B97+C97/60+D97/3600</f>
+        <v>30.456499999999998</v>
+      </c>
+      <c r="F97" s="1">
+        <v>89</v>
+      </c>
+      <c r="G97">
+        <v>47</v>
+      </c>
+      <c r="H97">
+        <v>5.2</v>
+      </c>
+      <c r="I97">
+        <f t="shared" ref="I97:I115" si="17">-F97-G97/60-H97/3600</f>
+        <v>-89.784777777777776</v>
+      </c>
+    </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B98" s="1">
         <v>30</v>
       </c>
       <c r="C98">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D98">
-        <v>23.4</v>
+        <v>48.4</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" ref="E98:E110" si="16">B98+C98/60+D98/3600</f>
-        <v>30.456499999999998</v>
+        <f t="shared" si="16"/>
+        <v>30.49677777777778</v>
       </c>
       <c r="F98" s="1">
         <v>89</v>
       </c>
       <c r="G98">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H98">
-        <v>5.2</v>
+        <v>52.1</v>
       </c>
       <c r="I98">
-        <f t="shared" ref="I98:I110" si="17">-F98-G98/60-H98/3600</f>
-        <v>-89.784777777777776</v>
+        <f t="shared" si="17"/>
+        <v>-89.814472222222221</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B99" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C99">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D99">
-        <v>48.4</v>
+        <v>20</v>
       </c>
       <c r="E99" s="4">
         <f t="shared" si="16"/>
-        <v>30.49677777777778</v>
+        <v>31.755555555555556</v>
       </c>
       <c r="F99" s="1">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G99">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="H99">
-        <v>52.1</v>
+        <v>13</v>
       </c>
       <c r="I99">
         <f t="shared" si="17"/>
-        <v>-89.814472222222221</v>
+        <v>-93.120277777777773</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B100" s="1">
         <v>31</v>
       </c>
       <c r="C100">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D100">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E100" s="4">
         <f t="shared" si="16"/>
-        <v>31.755555555555556</v>
+        <v>31.774444444444445</v>
       </c>
       <c r="F100" s="1">
         <v>93</v>
       </c>
       <c r="G100">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H100">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I100">
         <f t="shared" si="17"/>
-        <v>-93.120277777777773</v>
+        <v>-93.084722222222211</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C101">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E101" s="4">
         <f t="shared" si="16"/>
-        <v>31.774444444444445</v>
+        <v>32.00138888888889</v>
       </c>
       <c r="F101" s="1">
         <v>93</v>
       </c>
       <c r="G101">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H101">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I101">
         <f t="shared" si="17"/>
-        <v>-93.084722222222211</v>
+        <v>-93.269722222222228</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B102" s="1">
         <v>32</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D102">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E102" s="4">
         <f t="shared" si="16"/>
-        <v>32.00138888888889</v>
+        <v>32.700833333333335</v>
       </c>
       <c r="F102" s="1">
         <v>93</v>
       </c>
       <c r="G102">
+        <v>30</v>
+      </c>
+      <c r="H102">
         <v>16</v>
-      </c>
-      <c r="H102">
-        <v>11</v>
       </c>
       <c r="I102">
         <f t="shared" si="17"/>
-        <v>-93.269722222222228</v>
+        <v>-93.504444444444445</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B103" s="1">
         <v>32</v>
       </c>
       <c r="C103">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D103">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="E103" s="4">
         <f t="shared" si="16"/>
-        <v>32.700833333333335</v>
+        <v>32.848611111111111</v>
       </c>
       <c r="F103" s="1">
         <v>93</v>
       </c>
       <c r="G103">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H103">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I103">
         <f t="shared" si="17"/>
-        <v>-93.504444444444445</v>
+        <v>-93.520277777777778</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" s="1">
         <v>32</v>
       </c>
       <c r="C104">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D104">
-        <v>55</v>
+        <v>2.78</v>
       </c>
       <c r="E104" s="4">
         <f t="shared" si="16"/>
-        <v>32.848611111111111</v>
+        <v>32.734105555555558</v>
       </c>
       <c r="F104" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G104">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="H104">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I104">
         <f t="shared" si="17"/>
-        <v>-93.520277777777778</v>
+        <v>-92.937222222222232</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C105">
         <v>44</v>
       </c>
       <c r="D105">
-        <v>2.78</v>
+        <v>46</v>
       </c>
       <c r="E105" s="4">
         <f t="shared" si="16"/>
-        <v>32.734105555555558</v>
+        <v>31.746111111111112</v>
       </c>
       <c r="F105" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G105">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="H105">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="I105">
         <f t="shared" si="17"/>
-        <v>-92.937222222222232</v>
+        <v>-91.441666666666677</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1">
         <v>31</v>
       </c>
       <c r="C106">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D106">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E106" s="4">
         <f t="shared" si="16"/>
-        <v>31.746111111111112</v>
+        <v>31.973333333333333</v>
       </c>
       <c r="F106" s="1">
         <v>91</v>
       </c>
       <c r="G106">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H106">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I106">
         <f t="shared" si="17"/>
-        <v>-91.441666666666677</v>
+        <v>-91.226111111111109</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" s="1">
         <v>31</v>
       </c>
       <c r="C107">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D107">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E107" s="4">
         <f t="shared" si="16"/>
-        <v>31.973333333333333</v>
+        <v>31.483055555555556</v>
       </c>
       <c r="F107" s="1">
         <v>91</v>
       </c>
       <c r="G107">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="H107">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I107">
         <f t="shared" si="17"/>
-        <v>-91.226111111111109</v>
+        <v>-91.8611111111111</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1">
         <v>31</v>
       </c>
       <c r="C108">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D108">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="E108" s="4">
         <f t="shared" si="16"/>
-        <v>31.483055555555556</v>
+        <v>31.373333333333335</v>
       </c>
       <c r="F108" s="1">
         <v>91</v>
       </c>
       <c r="G108">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H108">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="I108">
         <f t="shared" si="17"/>
-        <v>-91.8611111111111</v>
+        <v>-91.905277777777783</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1">
         <v>31</v>
       </c>
       <c r="C109">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D109">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E109" s="4">
         <f t="shared" si="16"/>
-        <v>31.373333333333335</v>
+        <v>31.333888888888886</v>
       </c>
       <c r="F109" s="1">
         <v>91</v>
       </c>
       <c r="G109">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H109">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I109">
         <f t="shared" si="17"/>
-        <v>-91.905277777777783</v>
+        <v>-91.936388888888899</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>108</v>
+      <c r="A110" s="4">
+        <v>109</v>
       </c>
       <c r="B110" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C110">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>28.4</v>
       </c>
       <c r="E110" s="4">
         <f t="shared" si="16"/>
-        <v>31.333888888888886</v>
+        <v>30.457888888888888</v>
       </c>
       <c r="F110" s="1">
         <v>91</v>
       </c>
       <c r="G110">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="H110">
-        <v>11</v>
+        <v>53.4</v>
       </c>
       <c r="I110">
         <f t="shared" si="17"/>
-        <v>-91.936388888888899</v>
+        <v>-91.1815</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E111" s="4"/>
+      <c r="A111" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B111" s="1">
+        <v>30</v>
+      </c>
+      <c r="C111">
+        <v>25</v>
+      </c>
+      <c r="D111">
+        <v>25.5</v>
+      </c>
+      <c r="E111" s="4">
+        <f t="shared" si="16"/>
+        <v>30.423750000000002</v>
+      </c>
+      <c r="F111" s="1">
+        <v>91</v>
+      </c>
+      <c r="G111">
+        <v>10</v>
+      </c>
+      <c r="H111">
+        <v>5.7</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="17"/>
+        <v>-91.16825</v>
+      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E113" s="4"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E114" s="4"/>
+      <c r="A112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="1">
+        <v>30</v>
+      </c>
+      <c r="C112">
+        <v>25</v>
+      </c>
+      <c r="D112">
+        <v>50.3</v>
+      </c>
+      <c r="E112" s="4">
+        <f t="shared" si="16"/>
+        <v>30.43063888888889</v>
+      </c>
+      <c r="F112" s="1">
+        <v>91</v>
+      </c>
+      <c r="G112">
+        <v>10</v>
+      </c>
+      <c r="H112">
+        <v>6.4</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="17"/>
+        <v>-91.168444444444447</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" s="1">
+        <v>30</v>
+      </c>
+      <c r="C113">
+        <v>24</v>
+      </c>
+      <c r="D113">
+        <v>31.9</v>
+      </c>
+      <c r="E113" s="4">
+        <f t="shared" si="16"/>
+        <v>30.408861111111111</v>
+      </c>
+      <c r="F113" s="1">
+        <v>91</v>
+      </c>
+      <c r="G113">
+        <v>10</v>
+      </c>
+      <c r="H113">
+        <v>22.5</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="17"/>
+        <v>-91.172916666666666</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114" s="1">
+        <v>30</v>
+      </c>
+      <c r="C114">
+        <v>25</v>
+      </c>
+      <c r="D114">
+        <v>3.8</v>
+      </c>
+      <c r="E114" s="4">
+        <f t="shared" si="16"/>
+        <v>30.417722222222224</v>
+      </c>
+      <c r="F114" s="1">
+        <v>91</v>
+      </c>
+      <c r="G114">
+        <v>10</v>
+      </c>
+      <c r="H114">
+        <v>11.1</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="17"/>
+        <v>-91.169750000000008</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>110</v>
+      </c>
+      <c r="B115" s="1">
+        <v>29</v>
+      </c>
+      <c r="C115">
+        <v>49</v>
+      </c>
+      <c r="D115">
+        <v>26.658000000000001</v>
+      </c>
+      <c r="E115" s="4">
+        <f t="shared" si="16"/>
+        <v>29.824071666666665</v>
+      </c>
+      <c r="F115" s="1">
+        <v>90</v>
+      </c>
+      <c r="G115">
+        <v>28</v>
+      </c>
+      <c r="H115">
+        <v>33.603999999999999</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="17"/>
+        <v>-90.476001111111117</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>111</v>
+      </c>
+      <c r="B116" s="1">
+        <v>29</v>
+      </c>
+      <c r="C116">
+        <v>47</v>
+      </c>
+      <c r="D116">
+        <v>6</v>
+      </c>
+      <c r="E116" s="4">
+        <f t="shared" si="16"/>
+        <v>29.785</v>
+      </c>
+      <c r="F116" s="1">
+        <v>90</v>
+      </c>
+      <c r="G116">
+        <v>24</v>
+      </c>
+      <c r="H116">
+        <v>26.4</v>
+      </c>
+      <c r="I116">
+        <f>-F116-G116/60-H116/3600</f>
+        <v>-90.407333333333341</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>112</v>
+      </c>
+      <c r="B117" s="1">
+        <v>29</v>
+      </c>
+      <c r="C117">
+        <v>49</v>
+      </c>
+      <c r="D117">
+        <v>26.658000000000001</v>
+      </c>
+      <c r="E117" s="4">
+        <f>B117+C117/60+D117/3600</f>
+        <v>29.824071666666665</v>
+      </c>
+      <c r="F117" s="1">
+        <v>90</v>
+      </c>
+      <c r="G117">
+        <v>28</v>
+      </c>
+      <c r="H117">
+        <v>33.603999999999999</v>
+      </c>
+      <c r="I117">
+        <f>-F117-G117/60-H117/3600</f>
+        <v>-90.476001111111117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>113</v>
+      </c>
+      <c r="B118" s="1">
+        <v>29</v>
+      </c>
+      <c r="C118">
+        <v>38</v>
+      </c>
+      <c r="D118">
+        <v>48.4</v>
+      </c>
+      <c r="E118" s="4">
+        <f>B118+C118/60+D118/3600</f>
+        <v>29.646777777777778</v>
+      </c>
+      <c r="F118" s="1">
+        <v>90</v>
+      </c>
+      <c r="G118">
+        <v>32</v>
+      </c>
+      <c r="H118">
+        <v>27.4</v>
+      </c>
+      <c r="I118">
+        <f>-F118-G118/60-H118/3600</f>
+        <v>-90.540944444444449</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>114</v>
+      </c>
+      <c r="B119" s="1">
+        <v>29</v>
+      </c>
+      <c r="C119">
+        <v>52</v>
+      </c>
+      <c r="D119">
+        <v>0.3</v>
+      </c>
+      <c r="E119" s="4">
+        <f>B119+C119/60+D119/3600</f>
+        <v>29.86675</v>
+      </c>
+      <c r="F119" s="1">
+        <v>90</v>
+      </c>
+      <c r="G119">
+        <v>35</v>
+      </c>
+      <c r="H119">
+        <v>58.8</v>
+      </c>
+      <c r="I119">
+        <f>-F119-G119/60-H119/3600</f>
+        <v>-90.599666666666664</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4480,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4521,7 +4849,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -4531,11 +4859,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
-  <dimension ref="A1:S109"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L69" sqref="L69"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4599,10 +4927,10 @@
         <v>19</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -9721,16 +10049,16 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C93">
-        <v>30.456499999999998</v>
+        <v>29.86675</v>
       </c>
       <c r="D93">
-        <v>-89.784777777777776</v>
+        <v>-90.540947777777774</v>
       </c>
       <c r="E93" s="9">
         <v>0</v>
@@ -9772,7 +10100,7 @@
         <v>0</v>
       </c>
       <c r="R93" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93" s="9">
         <v>0</v>
@@ -9780,16 +10108,16 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C94">
-        <v>30.49677777777778</v>
+        <v>30.456499999999998</v>
       </c>
       <c r="D94">
-        <v>-89.814472222222221</v>
+        <v>-89.784777777777776</v>
       </c>
       <c r="E94" s="9">
         <v>0</v>
@@ -9819,19 +10147,19 @@
         <v>0</v>
       </c>
       <c r="N94" s="9">
+        <v>0</v>
+      </c>
+      <c r="O94" s="9">
+        <v>0</v>
+      </c>
+      <c r="P94" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="9">
+        <v>0</v>
+      </c>
+      <c r="R94" s="9">
         <v>1</v>
-      </c>
-      <c r="O94" s="9">
-        <v>0</v>
-      </c>
-      <c r="P94" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="9">
-        <v>0</v>
-      </c>
-      <c r="R94" s="9">
-        <v>0</v>
       </c>
       <c r="S94" s="9">
         <v>0</v>
@@ -9839,117 +10167,117 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C95">
-        <v>31.755555555555556</v>
+        <v>30.49677777777778</v>
       </c>
       <c r="D95">
-        <v>-93.120277777777773</v>
+        <v>-89.814472222222221</v>
+      </c>
+      <c r="E95" s="9">
+        <v>0</v>
+      </c>
+      <c r="F95" s="9">
+        <v>0</v>
+      </c>
+      <c r="G95" s="9">
+        <v>0</v>
+      </c>
+      <c r="H95" s="9">
+        <v>0</v>
+      </c>
+      <c r="I95" s="9">
+        <v>0</v>
+      </c>
+      <c r="J95" s="9">
+        <v>0</v>
+      </c>
+      <c r="K95" s="9">
+        <v>0</v>
+      </c>
+      <c r="L95" s="9">
+        <v>0</v>
+      </c>
+      <c r="M95" s="9">
+        <v>0</v>
+      </c>
+      <c r="N95" s="9">
+        <v>1</v>
+      </c>
+      <c r="O95" s="9">
+        <v>0</v>
+      </c>
+      <c r="P95" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="9">
+        <v>0</v>
+      </c>
+      <c r="R95" s="9">
+        <v>0</v>
+      </c>
+      <c r="S95" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C96">
-        <v>31.774444444444445</v>
+        <v>31.755555555555556</v>
       </c>
       <c r="D96">
-        <v>-93.084722222222211</v>
+        <v>-93.120277777777773</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C97">
-        <v>32.00138888888889</v>
+        <v>31.774444444444445</v>
       </c>
       <c r="D97">
-        <v>-93.269722222222228</v>
+        <v>-93.084722222222211</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C98">
-        <v>32.700833333333335</v>
+        <v>32.00138888888889</v>
       </c>
       <c r="D98">
-        <v>-93.504444444444445</v>
-      </c>
-      <c r="E98" s="9">
-        <v>0</v>
-      </c>
-      <c r="F98" s="9">
-        <v>0</v>
-      </c>
-      <c r="G98" s="9">
-        <v>0</v>
-      </c>
-      <c r="H98" s="9">
-        <v>0</v>
-      </c>
-      <c r="I98" s="9">
-        <v>0</v>
-      </c>
-      <c r="J98" s="9">
-        <v>0</v>
-      </c>
-      <c r="K98" s="9">
-        <v>0</v>
-      </c>
-      <c r="L98" s="9">
-        <v>12</v>
-      </c>
-      <c r="M98" s="9">
-        <v>0</v>
-      </c>
-      <c r="N98" s="9">
-        <v>0</v>
-      </c>
-      <c r="O98" s="9">
-        <v>0</v>
-      </c>
-      <c r="P98" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="9">
-        <v>0</v>
-      </c>
-      <c r="R98" s="9">
-        <v>0</v>
-      </c>
-      <c r="S98" s="9">
-        <v>0</v>
+        <v>-93.269722222222228</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C99">
-        <v>32.848611111111111</v>
+        <v>32.700833333333335</v>
       </c>
       <c r="D99">
-        <v>-93.520277777777778</v>
+        <v>-93.504444444444445</v>
       </c>
       <c r="E99" s="9">
         <v>0</v>
@@ -9973,7 +10301,7 @@
         <v>0</v>
       </c>
       <c r="L99" s="9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="M99" s="9">
         <v>0</v>
@@ -9982,7 +10310,7 @@
         <v>0</v>
       </c>
       <c r="O99" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P99" s="9">
         <v>0</v>
@@ -9999,16 +10327,16 @@
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C100">
-        <v>32.734105555555558</v>
+        <v>32.848611111111111</v>
       </c>
       <c r="D100">
-        <v>-92.937222222222232</v>
+        <v>-93.520277777777778</v>
       </c>
       <c r="E100" s="9">
         <v>0</v>
@@ -10041,7 +10369,7 @@
         <v>0</v>
       </c>
       <c r="O100" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P100" s="9">
         <v>0</v>
@@ -10058,134 +10386,191 @@
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C101">
-        <v>31.746111111111112</v>
+        <v>32.734105555555558</v>
       </c>
       <c r="D101">
-        <v>-91.441666666666677</v>
+        <v>-92.937222222222232</v>
+      </c>
+      <c r="E101" s="9">
+        <v>0</v>
+      </c>
+      <c r="F101" s="9">
+        <v>0</v>
+      </c>
+      <c r="G101" s="9">
+        <v>0</v>
+      </c>
+      <c r="H101" s="9">
+        <v>0</v>
+      </c>
+      <c r="I101" s="9">
+        <v>0</v>
+      </c>
+      <c r="J101" s="9">
+        <v>0</v>
+      </c>
+      <c r="K101" s="9">
+        <v>0</v>
+      </c>
+      <c r="L101" s="9">
+        <v>1</v>
+      </c>
+      <c r="M101" s="9">
+        <v>0</v>
+      </c>
+      <c r="N101" s="9">
+        <v>0</v>
+      </c>
+      <c r="O101" s="9">
+        <v>0</v>
+      </c>
+      <c r="P101" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="9">
+        <v>0</v>
+      </c>
+      <c r="R101" s="9">
+        <v>0</v>
+      </c>
+      <c r="S101" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C102">
-        <v>31.973333333333333</v>
+        <v>31.746111111111112</v>
       </c>
       <c r="D102">
-        <v>-91.226111111111109</v>
+        <v>-91.441666666666677</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C103">
-        <v>31.483055555555556</v>
+        <v>31.973333333333333</v>
       </c>
       <c r="D103">
-        <v>-91.8611111111111</v>
+        <v>-91.226111111111109</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C104">
-        <v>31.373333333333335</v>
+        <v>31.483055555555556</v>
       </c>
       <c r="D104">
-        <v>-91.905277777777783</v>
-      </c>
-      <c r="E104" s="9">
-        <v>0</v>
-      </c>
-      <c r="F104" s="9">
-        <v>0</v>
-      </c>
-      <c r="G104" s="9">
-        <v>0</v>
-      </c>
-      <c r="H104" s="9">
-        <v>0</v>
-      </c>
-      <c r="I104" s="9">
-        <v>0</v>
-      </c>
-      <c r="J104" s="9">
-        <v>0</v>
-      </c>
-      <c r="K104" s="9">
-        <v>0</v>
-      </c>
-      <c r="L104" s="9">
-        <v>0</v>
-      </c>
-      <c r="M104" s="9">
-        <v>0</v>
-      </c>
-      <c r="N104" s="9">
-        <v>0</v>
-      </c>
-      <c r="O104" s="9">
-        <v>0</v>
-      </c>
-      <c r="P104" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q104" s="9">
-        <v>0</v>
-      </c>
-      <c r="R104" s="9">
-        <v>0</v>
-      </c>
-      <c r="S104" s="9">
-        <v>0</v>
+        <v>-91.8611111111111</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105">
+        <v>107</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <v>31.373333333333335</v>
+      </c>
+      <c r="D105">
+        <v>-91.905277777777783</v>
+      </c>
+      <c r="E105" s="9">
+        <v>0</v>
+      </c>
+      <c r="F105" s="9">
+        <v>0</v>
+      </c>
+      <c r="G105" s="9">
+        <v>0</v>
+      </c>
+      <c r="H105" s="9">
+        <v>0</v>
+      </c>
+      <c r="I105" s="9">
+        <v>0</v>
+      </c>
+      <c r="J105" s="9">
+        <v>0</v>
+      </c>
+      <c r="K105" s="9">
+        <v>0</v>
+      </c>
+      <c r="L105" s="9">
+        <v>0</v>
+      </c>
+      <c r="M105" s="9">
+        <v>0</v>
+      </c>
+      <c r="N105" s="9">
+        <v>0</v>
+      </c>
+      <c r="O105" s="9">
+        <v>0</v>
+      </c>
+      <c r="P105" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="9">
+        <v>0</v>
+      </c>
+      <c r="R105" s="9">
+        <v>0</v>
+      </c>
+      <c r="S105" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A106">
         <v>108</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C105">
+      <c r="B106" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106">
         <v>31.333888888888886</v>
       </c>
-      <c r="D105">
+      <c r="D106">
         <v>-91.936388888888899</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
-        <v>24</v>
+      <c r="A107">
+        <v>109</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C107">
+        <v>30.457888888888888</v>
+      </c>
+      <c r="D107">
+        <v>-91.1815</v>
+      </c>
       <c r="E107" s="9">
         <v>0</v>
       </c>
@@ -10234,19 +10619,31 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="C108">
+        <v>30.423750000000002</v>
+      </c>
+      <c r="D108">
+        <v>-91.16825</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C109">
+        <v>30.43063888888889</v>
+      </c>
+      <c r="D109">
+        <v>-91.168444444444447</v>
+      </c>
       <c r="E109" s="9">
         <v>0</v>
       </c>
@@ -10291,6 +10688,149 @@
       </c>
       <c r="S109" s="9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>30.408861111111111</v>
+      </c>
+      <c r="D110">
+        <v>-91.172916666666666</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111">
+        <v>30.417722222222224</v>
+      </c>
+      <c r="D111">
+        <v>-91.169750000000008</v>
+      </c>
+      <c r="E111" s="9">
+        <v>0</v>
+      </c>
+      <c r="F111" s="9">
+        <v>0</v>
+      </c>
+      <c r="G111" s="9">
+        <v>0</v>
+      </c>
+      <c r="H111" s="9">
+        <v>0</v>
+      </c>
+      <c r="I111" s="9">
+        <v>0</v>
+      </c>
+      <c r="J111" s="9">
+        <v>0</v>
+      </c>
+      <c r="K111" s="9">
+        <v>0</v>
+      </c>
+      <c r="L111" s="9">
+        <v>0</v>
+      </c>
+      <c r="M111" s="9">
+        <v>0</v>
+      </c>
+      <c r="N111" s="9">
+        <v>0</v>
+      </c>
+      <c r="O111" s="9">
+        <v>0</v>
+      </c>
+      <c r="P111" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="9">
+        <v>0</v>
+      </c>
+      <c r="R111" s="9">
+        <v>0</v>
+      </c>
+      <c r="S111" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="D112">
+        <v>-90.476001111111117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113">
+        <v>29.785</v>
+      </c>
+      <c r="D113">
+        <v>-90.407333333333341</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="D114">
+        <v>-90.476001111111117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115">
+        <v>29.646777777777778</v>
+      </c>
+      <c r="D115">
+        <v>-90.540944444444449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>29.86675</v>
+      </c>
+      <c r="D116">
+        <v>-90.599666666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added light microscopy pictures
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBA00AE-FAB5-C44A-8390-79B06ECBA32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6E848-08BE-6640-A7CD-9957F38E880F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -4862,8 +4862,8 @@
   <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8921,7 +8921,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="10">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="M69" s="10">
         <v>0</v>
@@ -9371,21 +9371,51 @@
       <c r="D77">
         <v>-91.827305555555554</v>
       </c>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-      <c r="S77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S77" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78">

</xml_diff>

<commit_message>
Added more data to GPS coordinates to portray additional samples that have been found
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6E848-08BE-6640-A7CD-9957F38E880F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0774EA9-62D7-AC49-91F7-D028A3E574DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -4136,10 +4136,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76825C-C293-7549-99D8-78EF98420F3C}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4468,13 +4468,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B24">
-        <v>32.700833333333335</v>
+        <v>31.755555555555556</v>
       </c>
       <c r="C24">
-        <v>-93.504444444444445</v>
+        <v>-93.120277777777773</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -4482,13 +4482,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B25">
-        <v>32.848611111111111</v>
+        <v>32.00138888888889</v>
       </c>
       <c r="C25">
-        <v>-93.520277777777778</v>
+        <v>-93.269722222222228</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>3</v>
@@ -4496,15 +4496,85 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>100</v>
+      </c>
+      <c r="B26">
+        <v>32.700833333333335</v>
+      </c>
+      <c r="C26">
+        <v>-93.504444444444445</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>102</v>
+      </c>
+      <c r="B27">
+        <v>32.848611111111111</v>
+      </c>
+      <c r="C27">
+        <v>-93.520277777777778</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>103</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>32.734105555555558</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <v>-92.937222222222232</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>104</v>
+      </c>
+      <c r="B29">
+        <v>31.746111111111112</v>
+      </c>
+      <c r="C29">
+        <v>-91.441666666666677</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <v>30.423750000000002</v>
+      </c>
+      <c r="C30">
+        <v>-91.16825</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>30.408861111111111</v>
+      </c>
+      <c r="C31">
+        <v>-91.172916666666666</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4575,10 +4645,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C81C191-73FC-1D4C-874E-DD6089F6BB59}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4641,15 +4711,29 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>30.456499999999998</v>
+      </c>
+      <c r="C5">
+        <v>-89.784777777777776</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>96</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>30.49677777777778</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>-89.814472222222221</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4863,7 +4947,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6086,16 +6170,16 @@
         <v>0</v>
       </c>
       <c r="K21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="10">
+        <v>10</v>
+      </c>
+      <c r="M21" s="10">
+        <v>0</v>
+      </c>
+      <c r="N21" s="10">
         <v>8</v>
-      </c>
-      <c r="M21" s="10">
-        <v>0</v>
-      </c>
-      <c r="N21" s="10">
-        <v>6</v>
       </c>
       <c r="O21" s="10">
         <v>0</v>
@@ -6189,11 +6273,11 @@
         <v>0</v>
       </c>
       <c r="F23" s="10">
+        <v>7</v>
+      </c>
+      <c r="G23" s="10">
         <v>5</v>
       </c>
-      <c r="G23" s="10">
-        <v>4</v>
-      </c>
       <c r="H23" s="10">
         <v>0</v>
       </c>
@@ -6204,7 +6288,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="10">
         <v>9</v>
@@ -6440,10 +6524,10 @@
         <v>0</v>
       </c>
       <c r="K27" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L27" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M27" s="10">
         <v>0</v>
@@ -10153,7 +10237,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="9">
         <v>0</v>
@@ -10177,7 +10261,7 @@
         <v>0</v>
       </c>
       <c r="N94" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O94" s="9">
         <v>0</v>
@@ -10267,6 +10351,9 @@
       <c r="D96">
         <v>-93.120277777777773</v>
       </c>
+      <c r="L96" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
@@ -10281,6 +10368,9 @@
       <c r="D97">
         <v>-93.084722222222211</v>
       </c>
+      <c r="E97" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
@@ -10295,6 +10385,9 @@
       <c r="D98">
         <v>-93.269722222222228</v>
       </c>
+      <c r="L98" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
@@ -10331,7 +10424,7 @@
         <v>0</v>
       </c>
       <c r="L99" s="9">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M99" s="9">
         <v>0</v>
@@ -10390,7 +10483,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M100" s="9">
         <v>0</v>
@@ -10449,7 +10542,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M101" s="9">
         <v>0</v>
@@ -10486,6 +10579,9 @@
       <c r="D102">
         <v>-91.441666666666677</v>
       </c>
+      <c r="L102" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
@@ -10660,6 +10756,9 @@
       <c r="D108">
         <v>-91.16825</v>
       </c>
+      <c r="L108" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
@@ -10733,6 +10832,9 @@
       <c r="D110">
         <v>-91.172916666666666</v>
       </c>
+      <c r="L110" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
@@ -10806,8 +10908,14 @@
       <c r="D112">
         <v>-90.476001111111117</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112" s="9">
+        <v>1</v>
+      </c>
+      <c r="G112" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -10820,8 +10928,11 @@
       <c r="D113">
         <v>-90.407333333333341</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -10835,7 +10946,7 @@
         <v>-90.476001111111117</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -10849,7 +10960,7 @@
         <v>-90.540944444444449</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -10871,10 +10982,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0A8B15-BF5D-774F-B9D2-DF36EBC05789}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11039,6 +11150,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>98</v>
+      </c>
+      <c r="B12">
+        <v>31.774444444444445</v>
+      </c>
+      <c r="C12">
+        <v>-93.084722222222211</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="C13">
+        <v>-90.476001111111117</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>111</v>
+      </c>
+      <c r="B14">
+        <v>29.785</v>
+      </c>
+      <c r="C14">
+        <v>-90.407333333333341</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11047,10 +11200,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFEB945-8A1B-E94F-BD8C-E98A6236949A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11184,6 +11337,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>30.456499999999998</v>
+      </c>
+      <c r="C10">
+        <v>-89.784777777777776</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11191,10 +11358,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BE191B-F40C-4E42-8338-92AFBF23F2EB}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11583,6 +11750,20 @@
         <v>-91.97097222222223</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>110</v>
+      </c>
+      <c r="B28">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="C28">
+        <v>-90.476001111111117</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11825,10 +12006,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D622A2-17A0-C345-9A61-A2073C208DC6}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11863,13 +12044,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>31.878611111111113</v>
+        <v>32.140749999999997</v>
       </c>
       <c r="C3">
-        <v>-92.895833333333343</v>
+        <v>-93.593888888888884</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -11877,15 +12058,43 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>32.439166666666665</v>
+      </c>
+      <c r="C4">
+        <v>-93.37833333333333</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>31.878611111111113</v>
+      </c>
+      <c r="C5">
+        <v>-92.895833333333343</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>33</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>30.126750000000001</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>-91.27847222222222</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected data that is reflected on maps.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0774EA9-62D7-AC49-91F7-D028A3E574DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BF94ED-CB7E-5548-896C-83E17FADA297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -4947,7 +4947,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9291,7 +9291,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" s="10">
         <v>0</v>
@@ -11849,7 +11849,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11942,18 +11942,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>74</v>
-      </c>
-      <c r="B7">
-        <v>30.210333333333331</v>
-      </c>
-      <c r="C7">
-        <v>-92.001444444444445</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more data for maps.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BF94ED-CB7E-5548-896C-83E17FADA297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7281D5F-6043-B24F-B419-431BE9824A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="4" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -4136,10 +4136,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76825C-C293-7549-99D8-78EF98420F3C}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4578,6 +4578,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>112</v>
+      </c>
+      <c r="B32">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="C32">
+        <v>-90.476001111111117</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>114</v>
+      </c>
+      <c r="B33">
+        <v>29.86675</v>
+      </c>
+      <c r="C33">
+        <v>-90.599666666666664</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4585,10 +4613,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDF0D-3A19-D448-B6E0-DF89803F0E8E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4635,6 +4663,20 @@
         <v>-90.091555555555544</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>30.02547222222222</v>
+      </c>
+      <c r="C4">
+        <v>-90.115638888888881</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4945,9 +4987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
   <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115:D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5609,10 +5651,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>30.411805555555553</v>
@@ -6220,7 +6262,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I22" s="10">
         <v>1</v>
@@ -6229,10 +6271,10 @@
         <v>0</v>
       </c>
       <c r="K22" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M22" s="10">
         <v>0</v>
@@ -6273,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23" s="10">
         <v>5</v>
@@ -6288,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" s="10">
         <v>9</v>
@@ -6297,7 +6339,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O23" s="10">
         <v>0</v>
@@ -8090,7 +8132,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>30.480249999999998</v>
@@ -10116,7 +10158,7 @@
         <v>-90.115638888888881</v>
       </c>
       <c r="E92" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F92" s="9">
         <v>0</v>
@@ -10140,7 +10182,7 @@
         <v>0</v>
       </c>
       <c r="M92" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N92" s="9">
         <v>0</v>
@@ -10149,7 +10191,7 @@
         <v>0</v>
       </c>
       <c r="P92" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q92" s="9">
         <v>0</v>
@@ -10915,7 +10957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -10931,8 +10973,11 @@
       <c r="E113" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G113" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -10945,8 +10990,14 @@
       <c r="D114">
         <v>-90.476001111111117</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G114" s="9">
+        <v>10</v>
+      </c>
+      <c r="L114" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -10959,8 +11010,11 @@
       <c r="D115">
         <v>-90.540944444444449</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G115" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -10972,6 +11026,9 @@
       </c>
       <c r="D116">
         <v>-90.599666666666664</v>
+      </c>
+      <c r="L116" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10982,11 +11039,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0A8B15-BF5D-774F-B9D2-DF36EBC05789}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11152,13 +11207,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B12">
-        <v>31.774444444444445</v>
+        <v>30.02547222222222</v>
       </c>
       <c r="C12">
-        <v>-93.084722222222211</v>
+        <v>-90.115638888888881</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>3</v>
@@ -11166,13 +11221,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B13">
-        <v>29.824071666666665</v>
+        <v>31.774444444444445</v>
       </c>
       <c r="C13">
-        <v>-90.476001111111117</v>
+        <v>-93.084722222222211</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -11180,15 +11235,29 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="C14">
+        <v>-90.476001111111117</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>111</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>29.785</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>-90.407333333333341</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11358,10 +11427,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BE191B-F40C-4E42-8338-92AFBF23F2EB}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11755,15 +11824,57 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>111</v>
+      </c>
+      <c r="B28">
+        <v>29.785</v>
+      </c>
+      <c r="C28">
+        <v>-90.407333333333341</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>110</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>29.824071666666665</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>-90.476001111111117</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>112</v>
+      </c>
+      <c r="B30">
+        <v>29.824071666666665</v>
+      </c>
+      <c r="C30">
+        <v>-90.476001111111117</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>113</v>
+      </c>
+      <c r="B31">
+        <v>29.646777777777778</v>
+      </c>
+      <c r="C31">
+        <v>-90.540944444444449</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11997,10 +12108,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D622A2-17A0-C345-9A61-A2073C208DC6}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12035,13 +12146,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>32.140749999999997</v>
+        <v>32.32</v>
       </c>
       <c r="C3">
-        <v>-93.593888888888884</v>
+        <v>-93.67</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -12049,13 +12160,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>32.439166666666665</v>
+        <v>32.140749999999997</v>
       </c>
       <c r="C4">
-        <v>-93.37833333333333</v>
+        <v>-93.593888888888884</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -12063,13 +12174,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>31.878611111111113</v>
+        <v>32.439166666666665</v>
       </c>
       <c r="C5">
-        <v>-92.895833333333343</v>
+        <v>-93.37833333333333</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -12077,15 +12188,29 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>31.878611111111113</v>
+      </c>
+      <c r="C6">
+        <v>-92.895833333333343</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>33</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>30.126750000000001</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>-91.27847222222222</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited errors with GPS coordinates of some sites including duplicate ones.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7281D5F-6043-B24F-B419-431BE9824A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E111F3E-2427-5141-A235-EEEAEEC16BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="4" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AA6257-4E63-BE4C-BA67-DCDA03B0201E}">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView topLeftCell="C84" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +875,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>30</v>
@@ -887,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
+        <f>B12+C12/60+D12/3600</f>
         <v>30.818888888888889</v>
       </c>
       <c r="F12" s="1">
@@ -900,7 +900,7 @@
         <v>47</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f>-F12-G12/60-H12/3600</f>
         <v>-93.229722222222222</v>
       </c>
     </row>
@@ -2090,27 +2090,27 @@
         <v>30</v>
       </c>
       <c r="C51">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D51">
-        <v>42.5</v>
+        <v>14.4</v>
       </c>
       <c r="E51" s="4">
         <f t="shared" si="6"/>
-        <v>30.411805555555553</v>
+        <v>30.420666666666669</v>
       </c>
       <c r="F51" s="1">
         <v>90</v>
       </c>
       <c r="G51">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H51">
-        <v>32.6</v>
+        <v>48.7</v>
       </c>
       <c r="I51">
         <f t="shared" si="7"/>
-        <v>-90.142388888888902</v>
+        <v>-90.113527777777776</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2279,11 +2279,11 @@
         <v>46</v>
       </c>
       <c r="D57">
-        <v>1.2</v>
+        <v>49.4</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" ref="E57" si="8">B57+C57/60+D57/3600</f>
-        <v>30.766999999999999</v>
+        <f>B57+C57/60+D57/3600</f>
+        <v>30.780388888888886</v>
       </c>
       <c r="F57" s="1">
         <v>90</v>
@@ -2292,11 +2292,11 @@
         <v>8</v>
       </c>
       <c r="H57">
-        <v>40.5</v>
+        <v>55.1</v>
       </c>
       <c r="I57">
-        <f t="shared" ref="I57" si="9">-F57-G57/60-H57/3600</f>
-        <v>-90.144583333333344</v>
+        <f>-F57-G57/60-H57/3600</f>
+        <v>-90.148638888888897</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
         <v>43.1</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" ref="E58:E87" si="10">B58+C58/60+D58/3600</f>
+        <f t="shared" ref="E58:E87" si="8">B58+C58/60+D58/3600</f>
         <v>30.478638888888888</v>
       </c>
       <c r="F58" s="1">
@@ -2326,7 +2326,7 @@
         <v>36.9</v>
       </c>
       <c r="I58">
-        <f t="shared" ref="I58:I87" si="11">-F58-G58/60-H58/3600</f>
+        <f t="shared" ref="I58:I87" si="9">-F58-G58/60-H58/3600</f>
         <v>-90.993583333333333</v>
       </c>
     </row>
@@ -2344,7 +2344,7 @@
         <v>31.6</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.375444444444444</v>
       </c>
       <c r="F59" s="1">
@@ -2357,7 +2357,7 @@
         <v>20</v>
       </c>
       <c r="I59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-89.738888888888894</v>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
         <v>10.3</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.986194444444447</v>
       </c>
       <c r="F60" s="1">
@@ -2388,7 +2388,7 @@
         <v>12.4</v>
       </c>
       <c r="I60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-90.953444444444443</v>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
         <v>54.9</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.965250000000001</v>
       </c>
       <c r="F61" s="1">
@@ -2419,7 +2419,7 @@
         <v>43.5</v>
       </c>
       <c r="I61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.212083333333339</v>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
         <v>49.7</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.963805555555556</v>
       </c>
       <c r="F62" s="1">
@@ -2450,7 +2450,7 @@
         <v>38.5</v>
       </c>
       <c r="I62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.210694444444442</v>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.900305555555555</v>
       </c>
       <c r="F63" s="1">
@@ -2481,7 +2481,7 @@
         <v>9.1</v>
       </c>
       <c r="I63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.185861111111109</v>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.721416666666666</v>
       </c>
       <c r="F64" s="1">
@@ -2512,7 +2512,7 @@
         <v>23.4</v>
       </c>
       <c r="I64">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.18983333333334</v>
       </c>
     </row>
@@ -2530,7 +2530,7 @@
         <v>28.4</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.691222222222223</v>
       </c>
       <c r="F65" s="1">
@@ -2543,7 +2543,7 @@
         <v>54.2</v>
       </c>
       <c r="I65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.215055555555551</v>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.661305555555554</v>
       </c>
       <c r="F66" s="1">
@@ -2574,7 +2574,7 @@
         <v>38.9</v>
       </c>
       <c r="I66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.244138888888884</v>
       </c>
     </row>
@@ -2592,7 +2592,7 @@
         <v>35</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.693055555555556</v>
       </c>
       <c r="F67" s="1">
@@ -2605,7 +2605,7 @@
         <v>1.6</v>
       </c>
       <c r="I67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.433777777777777</v>
       </c>
     </row>
@@ -2623,7 +2623,7 @@
         <v>25.5</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.423750000000002</v>
       </c>
       <c r="F68" s="1">
@@ -2636,7 +2636,7 @@
         <v>5.7</v>
       </c>
       <c r="I68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.16825</v>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
         <v>29.6</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.458222222222222</v>
       </c>
       <c r="F69" s="1">
@@ -2667,7 +2667,7 @@
         <v>13.9</v>
       </c>
       <c r="I69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.187194444444444</v>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.126750000000001</v>
       </c>
       <c r="F70" s="1">
@@ -2698,7 +2698,7 @@
         <v>42.5</v>
       </c>
       <c r="I70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.27847222222222</v>
       </c>
     </row>
@@ -2716,7 +2716,7 @@
         <v>23.4</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.1065</v>
       </c>
       <c r="F71" s="1">
@@ -2729,7 +2729,7 @@
         <v>20.8</v>
       </c>
       <c r="I71">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-90.422444444444452</v>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
         <v>43.6</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.312111111111111</v>
       </c>
       <c r="F72" s="1">
@@ -2760,7 +2760,7 @@
         <v>18</v>
       </c>
       <c r="I72">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.788333333333327</v>
       </c>
     </row>
@@ -2778,7 +2778,7 @@
         <v>26.6</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.20738888888889</v>
       </c>
       <c r="F73" s="1">
@@ -2791,7 +2791,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="I73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-92.019499999999994</v>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.210333333333331</v>
       </c>
       <c r="F74" s="1">
@@ -2822,7 +2822,7 @@
         <v>5.2</v>
       </c>
       <c r="I74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-92.001444444444445</v>
       </c>
     </row>
@@ -2840,7 +2840,7 @@
         <v>59.5</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.216527777777777</v>
       </c>
       <c r="F75" s="1">
@@ -2853,7 +2853,7 @@
         <v>32.1</v>
       </c>
       <c r="I75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.992249999999999</v>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
         <v>13.2</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.203666666666667</v>
       </c>
       <c r="F76" s="1">
@@ -2884,7 +2884,7 @@
         <v>3.8</v>
       </c>
       <c r="I76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.901055555555558</v>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
         <v>18.7</v>
       </c>
       <c r="E77" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.121861111111112</v>
       </c>
       <c r="F77" s="1">
@@ -2915,7 +2915,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="I77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.827305555555554</v>
       </c>
     </row>
@@ -2933,7 +2933,7 @@
         <v>40.6</v>
       </c>
       <c r="E78" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.044611111111113</v>
       </c>
       <c r="F78" s="1">
@@ -2946,7 +2946,7 @@
         <v>45.8</v>
       </c>
       <c r="I78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.862722222222217</v>
       </c>
     </row>
@@ -2964,7 +2964,7 @@
         <v>36.9</v>
       </c>
       <c r="E79" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>31.010249999999999</v>
       </c>
       <c r="F79" s="1">
@@ -2977,7 +2977,7 @@
         <v>49.3</v>
       </c>
       <c r="I79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.64702777777778</v>
       </c>
     </row>
@@ -2995,7 +2995,7 @@
         <v>4</v>
       </c>
       <c r="E80" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>31.634444444444444</v>
       </c>
       <c r="F80" s="1">
@@ -3008,7 +3008,7 @@
         <v>40</v>
       </c>
       <c r="I80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.544444444444437</v>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
         <v>41.3</v>
       </c>
       <c r="E81" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.061472222222221</v>
       </c>
       <c r="F81" s="1">
@@ -3039,7 +3039,7 @@
         <v>31.1</v>
       </c>
       <c r="I81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.608638888888876</v>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
         <v>18.8</v>
       </c>
       <c r="E82" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>29.971888888888888</v>
       </c>
       <c r="F82" s="1">
@@ -3070,7 +3070,7 @@
         <v>15.5</v>
       </c>
       <c r="I82">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-91.97097222222223</v>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
         <v>13.5</v>
       </c>
       <c r="E86" s="4">
-        <f t="shared" ref="E86" si="12">B86+C86/60+D86/3600</f>
+        <f t="shared" ref="E86" si="10">B86+C86/60+D86/3600</f>
         <v>30.00375</v>
       </c>
       <c r="F86" s="1">
@@ -3132,7 +3132,7 @@
         <v>46.2</v>
       </c>
       <c r="I86">
-        <f t="shared" ref="I86" si="13">-F86-G86/60-H86/3600</f>
+        <f t="shared" ref="I86" si="11">-F86-G86/60-H86/3600</f>
         <v>-90.096166666666662</v>
       </c>
     </row>
@@ -3150,7 +3150,7 @@
         <v>33.9</v>
       </c>
       <c r="E87" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>30.409416666666665</v>
       </c>
       <c r="F87" s="1">
@@ -3163,7 +3163,7 @@
         <v>25.3</v>
       </c>
       <c r="I87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-90.140361111111119</v>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
         <v>59.7</v>
       </c>
       <c r="E88" s="4">
-        <f t="shared" ref="E88:E95" si="14">B88+C88/60+D88/3600</f>
+        <f t="shared" ref="E88:E95" si="12">B88+C88/60+D88/3600</f>
         <v>29.983249999999998</v>
       </c>
       <c r="F88" s="1">
@@ -3194,7 +3194,7 @@
         <v>25.1</v>
       </c>
       <c r="I88">
-        <f t="shared" ref="I88:I95" si="15">-F88-G88/60-H88/3600</f>
+        <f t="shared" ref="I88:I95" si="13">-F88-G88/60-H88/3600</f>
         <v>-90.090305555555545</v>
       </c>
     </row>
@@ -3212,7 +3212,7 @@
         <v>0.8</v>
       </c>
       <c r="E89" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>29.983555555555558</v>
       </c>
       <c r="F89" s="1">
@@ -3225,7 +3225,7 @@
         <v>28.9</v>
       </c>
       <c r="I89">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.091361111111112</v>
       </c>
     </row>
@@ -3243,7 +3243,7 @@
         <v>26.1</v>
       </c>
       <c r="E90" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>30.207249999999998</v>
       </c>
       <c r="F90" s="1">
@@ -3256,7 +3256,7 @@
         <v>21.7</v>
       </c>
       <c r="I90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.422694444444446</v>
       </c>
     </row>
@@ -3274,7 +3274,7 @@
         <v>53.5</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>30.031527777777775</v>
       </c>
       <c r="F91" s="1">
@@ -3287,7 +3287,7 @@
         <v>2.7</v>
       </c>
       <c r="I91">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.034083333333328</v>
       </c>
     </row>
@@ -3305,7 +3305,7 @@
         <v>23.3</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>30.539805555555557</v>
       </c>
       <c r="F92" s="1">
@@ -3318,7 +3318,7 @@
         <v>28.2</v>
       </c>
       <c r="I92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-89.874499999999998</v>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
         <v>27.9</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>30.024416666666667</v>
       </c>
       <c r="F93" s="1">
@@ -3349,7 +3349,7 @@
         <v>56.3</v>
       </c>
       <c r="I93">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.115638888888881</v>
       </c>
     </row>
@@ -3367,7 +3367,7 @@
         <v>31.7</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>30.02547222222222</v>
       </c>
       <c r="F94" s="1">
@@ -3380,7 +3380,7 @@
         <v>56.3</v>
       </c>
       <c r="I94">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.115638888888881</v>
       </c>
     </row>
@@ -3398,7 +3398,7 @@
         <v>0.3</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>29.86675</v>
       </c>
       <c r="F95" s="1">
@@ -3411,7 +3411,7 @@
         <v>27.411999999999999</v>
       </c>
       <c r="I95">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-90.540947777777774</v>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
         <v>23.4</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" ref="E97:E116" si="16">B97+C97/60+D97/3600</f>
+        <f t="shared" ref="E97:E116" si="14">B97+C97/60+D97/3600</f>
         <v>30.456499999999998</v>
       </c>
       <c r="F97" s="1">
@@ -3442,7 +3442,7 @@
         <v>5.2</v>
       </c>
       <c r="I97">
-        <f t="shared" ref="I97:I115" si="17">-F97-G97/60-H97/3600</f>
+        <f t="shared" ref="I97:I115" si="15">-F97-G97/60-H97/3600</f>
         <v>-89.784777777777776</v>
       </c>
     </row>
@@ -3460,7 +3460,7 @@
         <v>48.4</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.49677777777778</v>
       </c>
       <c r="F98" s="1">
@@ -3473,7 +3473,7 @@
         <v>52.1</v>
       </c>
       <c r="I98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-89.814472222222221</v>
       </c>
     </row>
@@ -3491,7 +3491,7 @@
         <v>20</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.755555555555556</v>
       </c>
       <c r="F99" s="1">
@@ -3504,7 +3504,7 @@
         <v>13</v>
       </c>
       <c r="I99">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-93.120277777777773</v>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
         <v>28</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.774444444444445</v>
       </c>
       <c r="F100" s="1">
@@ -3535,7 +3535,7 @@
         <v>5</v>
       </c>
       <c r="I100">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-93.084722222222211</v>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
         <v>5</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>32.00138888888889</v>
       </c>
       <c r="F101" s="1">
@@ -3566,7 +3566,7 @@
         <v>11</v>
       </c>
       <c r="I101">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-93.269722222222228</v>
       </c>
     </row>
@@ -3584,7 +3584,7 @@
         <v>3</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>32.700833333333335</v>
       </c>
       <c r="F102" s="1">
@@ -3597,7 +3597,7 @@
         <v>16</v>
       </c>
       <c r="I102">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-93.504444444444445</v>
       </c>
     </row>
@@ -3615,7 +3615,7 @@
         <v>55</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>32.848611111111111</v>
       </c>
       <c r="F103" s="1">
@@ -3628,7 +3628,7 @@
         <v>13</v>
       </c>
       <c r="I103">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-93.520277777777778</v>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
         <v>2.78</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>32.734105555555558</v>
       </c>
       <c r="F104" s="1">
@@ -3659,7 +3659,7 @@
         <v>14</v>
       </c>
       <c r="I104">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-92.937222222222232</v>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
         <v>46</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.746111111111112</v>
       </c>
       <c r="F105" s="1">
@@ -3690,7 +3690,7 @@
         <v>30</v>
       </c>
       <c r="I105">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.441666666666677</v>
       </c>
     </row>
@@ -3708,7 +3708,7 @@
         <v>24</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.973333333333333</v>
       </c>
       <c r="F106" s="1">
@@ -3721,7 +3721,7 @@
         <v>34</v>
       </c>
       <c r="I106">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.226111111111109</v>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
         <v>59</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.483055555555556</v>
       </c>
       <c r="F107" s="1">
@@ -3752,7 +3752,7 @@
         <v>40</v>
       </c>
       <c r="I107">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.8611111111111</v>
       </c>
     </row>
@@ -3770,7 +3770,7 @@
         <v>24</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.373333333333335</v>
       </c>
       <c r="F108" s="1">
@@ -3783,7 +3783,7 @@
         <v>19</v>
       </c>
       <c r="I108">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.905277777777783</v>
       </c>
     </row>
@@ -3801,7 +3801,7 @@
         <v>2</v>
       </c>
       <c r="E109" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>31.333888888888886</v>
       </c>
       <c r="F109" s="1">
@@ -3814,7 +3814,7 @@
         <v>11</v>
       </c>
       <c r="I109">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.936388888888899</v>
       </c>
     </row>
@@ -3832,7 +3832,7 @@
         <v>28.4</v>
       </c>
       <c r="E110" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.457888888888888</v>
       </c>
       <c r="F110" s="1">
@@ -3845,7 +3845,7 @@
         <v>53.4</v>
       </c>
       <c r="I110">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.1815</v>
       </c>
     </row>
@@ -3863,7 +3863,7 @@
         <v>25.5</v>
       </c>
       <c r="E111" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.423750000000002</v>
       </c>
       <c r="F111" s="1">
@@ -3876,7 +3876,7 @@
         <v>5.7</v>
       </c>
       <c r="I111">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.16825</v>
       </c>
     </row>
@@ -3894,7 +3894,7 @@
         <v>50.3</v>
       </c>
       <c r="E112" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.43063888888889</v>
       </c>
       <c r="F112" s="1">
@@ -3907,7 +3907,7 @@
         <v>6.4</v>
       </c>
       <c r="I112">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.168444444444447</v>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
         <v>31.9</v>
       </c>
       <c r="E113" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.408861111111111</v>
       </c>
       <c r="F113" s="1">
@@ -3938,7 +3938,7 @@
         <v>22.5</v>
       </c>
       <c r="I113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.172916666666666</v>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
         <v>3.8</v>
       </c>
       <c r="E114" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30.417722222222224</v>
       </c>
       <c r="F114" s="1">
@@ -3969,7 +3969,7 @@
         <v>11.1</v>
       </c>
       <c r="I114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-91.169750000000008</v>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
         <v>26.658000000000001</v>
       </c>
       <c r="E115" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>29.824071666666665</v>
       </c>
       <c r="F115" s="1">
@@ -4000,7 +4000,7 @@
         <v>33.603999999999999</v>
       </c>
       <c r="I115">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-90.476001111111117</v>
       </c>
     </row>
@@ -4018,7 +4018,7 @@
         <v>6</v>
       </c>
       <c r="E116" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>29.785</v>
       </c>
       <c r="F116" s="1">
@@ -4043,27 +4043,27 @@
         <v>29</v>
       </c>
       <c r="C117">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D117">
-        <v>26.658000000000001</v>
+        <v>15.3</v>
       </c>
       <c r="E117" s="4">
         <f>B117+C117/60+D117/3600</f>
-        <v>29.824071666666665</v>
+        <v>29.737583333333333</v>
       </c>
       <c r="F117" s="1">
         <v>90</v>
       </c>
       <c r="G117">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H117">
-        <v>33.603999999999999</v>
+        <v>50.4</v>
       </c>
       <c r="I117">
         <f>-F117-G117/60-H117/3600</f>
-        <v>-90.476001111111117</v>
+        <v>-90.647333333333336</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -4139,7 +4139,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4317,10 +4317,10 @@
         <v>51</v>
       </c>
       <c r="B13">
-        <v>30.411805555555553</v>
+        <v>30.420666666666669</v>
       </c>
       <c r="C13">
-        <v>-90.142388888888902</v>
+        <v>-90.113527777777776</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -4583,10 +4583,10 @@
         <v>112</v>
       </c>
       <c r="B32">
-        <v>29.824071666666665</v>
+        <v>29.737583333333333</v>
       </c>
       <c r="C32">
-        <v>-90.476001111111117</v>
+        <v>-90.647333333333336</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>3</v>
@@ -4987,9 +4987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
   <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115:D115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L114" sqref="L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5657,10 +5657,10 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>30.411805555555553</v>
+        <v>30.818888888888889</v>
       </c>
       <c r="D12">
-        <v>-90.142388888888902</v>
+        <v>-93.229722222222222</v>
       </c>
       <c r="E12" s="10">
         <v>0</v>
@@ -7958,10 +7958,10 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>30.411805555555553</v>
+        <v>30.420666666666669</v>
       </c>
       <c r="D51">
-        <v>-90.142388888888902</v>
+        <v>-90.113527777777776</v>
       </c>
       <c r="E51" s="10">
         <v>0</v>
@@ -8312,10 +8312,10 @@
         <v>3</v>
       </c>
       <c r="C57">
-        <v>30.766999999999999</v>
+        <v>30.780388888888886</v>
       </c>
       <c r="D57">
-        <v>-90.144583333333344</v>
+        <v>-90.148638888888897</v>
       </c>
       <c r="E57" s="10">
         <v>0</v>
@@ -10985,10 +10985,10 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>29.824071666666665</v>
+        <v>29.737583333333333</v>
       </c>
       <c r="D114">
-        <v>-90.476001111111117</v>
+        <v>-90.647333333333336</v>
       </c>
       <c r="G114" s="9">
         <v>10</v>
@@ -11429,8 +11429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BE191B-F40C-4E42-8338-92AFBF23F2EB}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11739,11 +11739,11 @@
       <c r="A22" s="4">
         <v>51</v>
       </c>
-      <c r="B22" s="4">
-        <v>30.411805555555553</v>
-      </c>
-      <c r="C22" s="4">
-        <v>-90.142388888888902</v>
+      <c r="B22">
+        <v>30.420666666666669</v>
+      </c>
+      <c r="C22">
+        <v>-90.113527777777776</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -11753,11 +11753,11 @@
       <c r="A23" s="4">
         <v>57</v>
       </c>
-      <c r="B23" s="4">
-        <v>30.766999999999999</v>
-      </c>
-      <c r="C23" s="4">
-        <v>-90.144583333333344</v>
+      <c r="B23">
+        <v>30.780388888888886</v>
+      </c>
+      <c r="C23">
+        <v>-90.148638888888897</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -11855,10 +11855,10 @@
         <v>112</v>
       </c>
       <c r="B30">
-        <v>29.824071666666665</v>
+        <v>29.737583333333333</v>
       </c>
       <c r="C30">
-        <v>-90.476001111111117</v>
+        <v>-90.647333333333336</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added more sites to Efr and Th maps.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E111F3E-2427-5141-A235-EEEAEEC16BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E84960-641A-F648-93A9-55AA947FDE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -4136,10 +4136,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D76825C-C293-7549-99D8-78EF98420F3C}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C32"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4594,15 +4594,29 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>113</v>
+      </c>
+      <c r="B33">
+        <v>29.646777777777778</v>
+      </c>
+      <c r="C33">
+        <v>-90.540944444444449</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>114</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>29.86675</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>-90.599666666666664</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4988,8 +5002,8 @@
   <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L114" sqref="L114"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6265,7 +6279,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J22" s="10">
         <v>0</v>
@@ -6274,7 +6288,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="10">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M22" s="10">
         <v>0</v>
@@ -11013,6 +11027,9 @@
       <c r="G115" s="9">
         <v>1</v>
       </c>
+      <c r="L115" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116">
@@ -11027,8 +11044,11 @@
       <c r="D116">
         <v>-90.599666666666664</v>
       </c>
+      <c r="G116" s="9">
+        <v>1</v>
+      </c>
       <c r="L116" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -11427,10 +11447,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BE191B-F40C-4E42-8338-92AFBF23F2EB}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11875,6 +11895,20 @@
         <v>-90.540944444444449</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>114</v>
+      </c>
+      <c r="B32">
+        <v>29.86675</v>
+      </c>
+      <c r="C32">
+        <v>-90.599666666666664</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated S. lacustris SEM picture.
</commit_message>
<xml_diff>
--- a/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
+++ b/map_data_files/Miller_sponge gps coordinates_summer 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E84960-641A-F648-93A9-55AA947FDE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C92878-A3ED-AC4E-977A-B4CEB95FA355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="26">
   <si>
     <t>Long</t>
   </si>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AA6257-4E63-BE4C-BA67-DCDA03B0201E}">
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117"/>
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4126,6 +4126,11 @@
       <c r="I119">
         <f>-F119-G119/60-H119/3600</f>
         <v>-90.599666666666664</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4999,11 +5004,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
-  <dimension ref="A1:S116"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F121" sqref="F121"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11049,6 +11054,34 @@
       </c>
       <c r="L116" s="9">
         <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <v>30.534781739361001</v>
+      </c>
+      <c r="D117">
+        <v>-91.087264372120899</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118">
+        <v>30.534781739361001</v>
+      </c>
+      <c r="D118">
+        <v>-91.087264372120899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>